<commit_message>
flutter app update, odk-x form update and rename of project
ODK-X app name change to 'FijiNetwork'
ODK-X forms updated - various
ccSocial Flutter app updated to reflect change to ODK app name
etc
</commit_message>
<xml_diff>
--- a/ODK-X_surveys/app/config/tables/household_member/forms/household_member/household_member.xlsx
+++ b/ODK-X_surveys/app/config/tables/household_member/forms/household_member/household_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="162">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -138,12 +138,6 @@
   </si>
   <si>
     <t xml:space="preserve">Kai Loma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">relationships</t>
@@ -1085,11 +1079,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.83"/>
@@ -1150,7 +1144,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.22"/>
@@ -1282,11 +1276,11 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
@@ -1414,15 +1408,9 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>38</v>
-      </c>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
@@ -1431,213 +1419,213 @@
     </row>
     <row r="15" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -1651,65 +1639,65 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -1749,7 +1737,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.49"/>
@@ -1758,10 +1746,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>21</v>
@@ -1769,16 +1757,16 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>2</v>
@@ -1787,16 +1775,16 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -1805,29 +1793,29 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1840,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.33"/>
@@ -1877,40 +1865,40 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,52 +1907,52 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,12 +1968,12 @@
         <v>28</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -1993,60 +1981,60 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
       <c r="B17" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28"/>
       <c r="B18" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28"/>
       <c r="B19" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28"/>
       <c r="B20" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28"/>
       <c r="B21" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28"/>
       <c r="B22" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2054,10 +2042,10 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,31 +2054,31 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28"/>
       <c r="B28" s="28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="30"/>
       <c r="B29" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2118,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.00390625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.03125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.55"/>
   </cols>
@@ -2168,7 +2156,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34"/>
       <c r="B2" s="34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
@@ -2184,12 +2172,12 @@
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
       <c r="G3" s="35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H3" s="35"/>
       <c r="I3" s="35"/>
@@ -2200,14 +2188,14 @@
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -2218,14 +2206,14 @@
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
       <c r="D5" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
@@ -2236,14 +2224,14 @@
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
       <c r="D6" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="36"/>
       <c r="F6" s="36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -2254,12 +2242,12 @@
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
       <c r="D7" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="36"/>
       <c r="G7" s="37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -2270,14 +2258,14 @@
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
       <c r="D8" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E8" s="36"/>
       <c r="F8" s="36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -2288,14 +2276,14 @@
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
       <c r="D9" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E9" s="36"/>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -2306,16 +2294,16 @@
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
@@ -2324,7 +2312,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="38"/>
       <c r="B11" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -2350,7 +2338,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
       <c r="B13" s="39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -2366,12 +2354,12 @@
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
       <c r="G14" s="39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
@@ -2382,7 +2370,7 @@
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E15" s="39" t="s">
         <v>28</v>
@@ -2391,7 +2379,7 @@
         <v>28</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
@@ -2400,7 +2388,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -2425,7 +2413,7 @@
     </row>
     <row r="18" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2434,18 +2422,18 @@
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J18" s="41"/>
     </row>
     <row r="19" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2454,12 +2442,12 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J19" s="41"/>
     </row>
@@ -2478,7 +2466,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38"/>
       <c r="B21" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -2494,16 +2482,16 @@
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E22" s="42" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
@@ -2514,14 +2502,14 @@
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E23" s="42"/>
       <c r="F23" s="42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H23" s="42"/>
       <c r="I23" s="42"/>
@@ -2532,16 +2520,16 @@
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E24" s="44" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G24" s="45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H24" s="39"/>
       <c r="I24" s="46"/>
@@ -2551,7 +2539,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -2584,7 +2572,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.95703125" defaultRowHeight="31" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="26.9921875" defaultRowHeight="31" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.5"/>
@@ -2623,7 +2611,7 @@
     <row r="2" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="49"/>
       <c r="B2" s="49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="50"/>
@@ -2649,16 +2637,16 @@
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
       <c r="D4" s="54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -2668,14 +2656,14 @@
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G5" s="56" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
@@ -2683,10 +2671,10 @@
     <row r="6" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="35"/>
       <c r="B6" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
@@ -2694,7 +2682,7 @@
       <c r="G6" s="37"/>
       <c r="H6" s="35"/>
       <c r="I6" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2702,16 +2690,16 @@
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -2719,7 +2707,7 @@
     <row r="8" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
       <c r="B8" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
@@ -2743,10 +2731,10 @@
     <row r="10" s="16" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="53"/>
       <c r="B10" s="53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D10" s="53"/>
       <c r="E10" s="53"/>
@@ -2760,14 +2748,14 @@
       <c r="B11" s="53"/>
       <c r="C11" s="53"/>
       <c r="D11" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H11" s="53"/>
       <c r="I11" s="53"/>
@@ -2775,7 +2763,7 @@
     <row r="12" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="53"/>
       <c r="B12" s="53" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
@@ -2788,10 +2776,10 @@
     <row r="14" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="56"/>
       <c r="B14" s="56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D14" s="56"/>
       <c r="E14" s="56"/>
@@ -2799,7 +2787,7 @@
       <c r="G14" s="56"/>
       <c r="H14" s="56"/>
       <c r="I14" s="56" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2807,16 +2795,16 @@
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
       <c r="D15" s="56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G15" s="56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
@@ -2824,7 +2812,7 @@
     <row r="16" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="56"/>
       <c r="B16" s="56" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="56"/>
@@ -2848,7 +2836,7 @@
     <row r="18" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="58"/>
       <c r="B18" s="49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" s="58"/>
       <c r="D18" s="58"/>
@@ -2864,7 +2852,7 @@
     <row r="20" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2879,14 +2867,14 @@
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
       <c r="D21" s="57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E21" s="57"/>
       <c r="F21" s="57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H21" s="35"/>
       <c r="I21" s="35"/>
@@ -2894,7 +2882,7 @@
     <row r="22" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2926,7 +2914,7 @@
       <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
@@ -2943,28 +2931,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="E1" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="F1" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="G1" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="H1" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="I1" s="62" t="s">
         <v>161</v>
-      </c>
-      <c r="H1" s="61" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" s="62" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>